<commit_message>
Get data for TOP20 whole year
</commit_message>
<xml_diff>
--- a/Week_Settings_DB.xlsx
+++ b/Week_Settings_DB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Project\Weekly-Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FC2CA0C-B53A-4AAF-B1C6-EC37E9AE265F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1FBBD41-4302-4C06-A862-1A4A3A7792B3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4DBF33FA-BF1C-47DC-ACE3-B863258BACB6}"/>
   </bookViews>
@@ -417,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2C6775B-5349-4E6E-91AA-63F7F78CEA04}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,15 +506,44 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>5</v>
+        <f>A6+1</f>
+        <v>6</v>
       </c>
       <c r="B7" s="1">
-        <f t="shared" ref="B7" si="1">B6+7</f>
+        <f t="shared" ref="B7:B9" si="1">B6+7</f>
         <v>43496</v>
       </c>
       <c r="C7" s="1">
-        <f t="shared" ref="C7" si="2">C6+7</f>
+        <f t="shared" ref="C7:C9" si="2">C6+7</f>
         <v>43502</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f>A7+1</f>
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <f t="shared" si="1"/>
+        <v>43503</v>
+      </c>
+      <c r="C8" s="1">
+        <f t="shared" si="2"/>
+        <v>43509</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f>A8+1</f>
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <f t="shared" si="1"/>
+        <v>43510</v>
+      </c>
+      <c r="C9" s="1">
+        <f t="shared" si="2"/>
+        <v>43516</v>
       </c>
     </row>
   </sheetData>

</xml_diff>